<commit_message>
Final update: * code cleanup * README file update
</commit_message>
<xml_diff>
--- a/src/utils/region_aggregates.xlsx
+++ b/src/utils/region_aggregates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilie.allen\PycharmProjects\long-term-gdp-model\src\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FA1EA6-51FA-4267-B26A-5E0C1F2A03B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6B2740-3120-4672-A3B9-9A9EBA123D31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{2089EA31-CDD8-45CF-927E-7F1EBEE26E8B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2089EA31-CDD8-45CF-927E-7F1EBEE26E8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_changes" sheetId="4" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">new_list!$A$1:$E$184</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2569,27 +2570,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259F9AA6-75E5-457F-98CC-C5C07F6AB414}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="5.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1"/>
+    <col min="14" max="14" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="144" t="s">
         <v>458</v>
       </c>
@@ -2613,7 +2614,7 @@
       <c r="O1" s="152"/>
       <c r="P1" s="42"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="141" t="s">
         <v>6</v>
       </c>
@@ -2655,7 +2656,7 @@
       </c>
       <c r="P2" s="42"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="130" t="s">
         <v>209</v>
       </c>
@@ -2697,7 +2698,7 @@
       </c>
       <c r="P3" s="42"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="130" t="s">
         <v>339</v>
       </c>
@@ -2739,7 +2740,7 @@
       </c>
       <c r="P4" s="42"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="130" t="s">
         <v>381</v>
       </c>
@@ -2781,7 +2782,7 @@
       </c>
       <c r="P5" s="42"/>
     </row>
-    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="130" t="s">
         <v>119</v>
       </c>
@@ -2829,7 +2830,7 @@
       <c r="V6" s="129"/>
       <c r="W6" s="129"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="130" t="s">
         <v>446</v>
       </c>
@@ -2859,7 +2860,7 @@
       </c>
       <c r="P7" s="42"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="130" t="s">
         <v>287</v>
       </c>
@@ -2889,7 +2890,7 @@
       </c>
       <c r="P8" s="42"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="130" t="s">
         <v>319</v>
       </c>
@@ -2919,7 +2920,7 @@
       </c>
       <c r="P9" s="42"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="130" t="s">
         <v>323</v>
       </c>
@@ -2949,7 +2950,7 @@
       </c>
       <c r="P10" s="42"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="130" t="s">
         <v>351</v>
       </c>
@@ -2980,7 +2981,7 @@
       </c>
       <c r="P11" s="42"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="130" t="s">
         <v>89</v>
       </c>
@@ -3011,7 +3012,7 @@
       </c>
       <c r="P12" s="42"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="132" t="s">
         <v>375</v>
       </c>
@@ -3042,7 +3043,7 @@
       </c>
       <c r="P13" s="42"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="42"/>
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
@@ -3065,7 +3066,7 @@
       </c>
       <c r="P14" s="42"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K15" s="130" t="s">
         <v>179</v>
       </c>
@@ -3084,7 +3085,7 @@
       </c>
       <c r="P15" s="42"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K16" s="130" t="s">
         <v>177</v>
       </c>
@@ -3103,7 +3104,7 @@
       </c>
       <c r="P16" s="42"/>
     </row>
-    <row r="17" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K17" s="130" t="s">
         <v>173</v>
       </c>
@@ -3122,7 +3123,7 @@
       </c>
       <c r="P17" s="42"/>
     </row>
-    <row r="18" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K18" s="130" t="s">
         <v>181</v>
       </c>
@@ -3141,7 +3142,7 @@
       </c>
       <c r="P18" s="42"/>
     </row>
-    <row r="19" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K19" s="130" t="s">
         <v>193</v>
       </c>
@@ -3160,7 +3161,7 @@
       </c>
       <c r="P19" s="42"/>
     </row>
-    <row r="20" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K20" s="130" t="s">
         <v>225</v>
       </c>
@@ -3179,7 +3180,7 @@
       </c>
       <c r="P20" s="42"/>
     </row>
-    <row r="21" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K21" s="130" t="s">
         <v>221</v>
       </c>
@@ -3198,7 +3199,7 @@
       </c>
       <c r="P21" s="42"/>
     </row>
-    <row r="22" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K22" s="130" t="s">
         <v>223</v>
       </c>
@@ -3216,7 +3217,7 @@
         <v>Europe</v>
       </c>
     </row>
-    <row r="23" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K23" s="130" t="s">
         <v>245</v>
       </c>
@@ -3234,7 +3235,7 @@
         <v>Asia-Pacific</v>
       </c>
     </row>
-    <row r="24" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K24" s="130" t="s">
         <v>293</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>Europe</v>
       </c>
     </row>
-    <row r="25" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K25" s="130" t="s">
         <v>329</v>
       </c>
@@ -3270,7 +3271,7 @@
         <v>Europe</v>
       </c>
     </row>
-    <row r="26" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K26" s="130" t="s">
         <v>191</v>
       </c>
@@ -3288,7 +3289,7 @@
         <v>FSU</v>
       </c>
     </row>
-    <row r="27" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K27" s="130" t="s">
         <v>97</v>
       </c>
@@ -3306,7 +3307,7 @@
         <v>Latin America</v>
       </c>
     </row>
-    <row r="28" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="11:16" x14ac:dyDescent="0.35">
       <c r="K28" s="130" t="s">
         <v>331</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>Europe</v>
       </c>
     </row>
-    <row r="29" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="11:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K29" s="132" t="s">
         <v>217</v>
       </c>
@@ -3361,20 +3362,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A8934B-B2B3-4DAE-B9B6-BE23DD16129C}">
   <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H136" sqref="H136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31" style="128" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.7109375" style="128"/>
-    <col min="4" max="4" width="13.42578125" style="129" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="129" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.7265625" style="128"/>
+    <col min="4" max="4" width="13.453125" style="129" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" style="129" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
@@ -3394,7 +3395,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
         <v>12</v>
       </c>
@@ -3414,7 +3415,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>114</v>
       </c>
@@ -3434,7 +3435,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
         <v>118</v>
       </c>
@@ -3454,7 +3455,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="47" t="s">
         <v>126</v>
       </c>
@@ -3475,7 +3476,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="47" t="s">
         <v>142</v>
       </c>
@@ -3496,7 +3497,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="47" t="s">
         <v>194</v>
       </c>
@@ -3517,7 +3518,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="47" t="s">
         <v>214</v>
       </c>
@@ -3537,7 +3538,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
         <v>228</v>
       </c>
@@ -3557,7 +3558,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="47" t="s">
         <v>266</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
         <v>358</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="49" t="s">
         <v>437</v>
       </c>
@@ -3617,7 +3618,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="51" t="s">
         <v>34</v>
       </c>
@@ -3635,7 +3636,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="51" t="s">
         <v>40</v>
       </c>
@@ -3653,7 +3654,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="51" t="s">
         <v>406</v>
       </c>
@@ -3671,7 +3672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="51" t="s">
         <v>72</v>
       </c>
@@ -3689,7 +3690,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="51" t="s">
         <v>408</v>
       </c>
@@ -3707,7 +3708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="51" t="s">
         <v>419</v>
       </c>
@@ -3725,7 +3726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="51" t="s">
         <v>86</v>
       </c>
@@ -3743,7 +3744,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="51" t="s">
         <v>409</v>
       </c>
@@ -3761,7 +3762,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="51" t="s">
         <v>94</v>
       </c>
@@ -3779,7 +3780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="51" t="s">
         <v>407</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="51" t="s">
         <v>106</v>
       </c>
@@ -3815,7 +3816,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="51" t="s">
         <v>136</v>
       </c>
@@ -3833,7 +3834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="51" t="s">
         <v>144</v>
       </c>
@@ -3851,7 +3852,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="51" t="s">
         <v>416</v>
       </c>
@@ -3869,7 +3870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="51" t="s">
         <v>148</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="51" t="s">
         <v>414</v>
       </c>
@@ -3905,7 +3906,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="51" t="s">
         <v>212</v>
       </c>
@@ -3923,7 +3924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="51" t="s">
         <v>220</v>
       </c>
@@ -3941,7 +3942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="51" t="s">
         <v>232</v>
       </c>
@@ -3959,7 +3960,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="51" t="s">
         <v>242</v>
       </c>
@@ -3977,7 +3978,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="51" t="s">
         <v>252</v>
       </c>
@@ -3995,7 +3996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="51" t="s">
         <v>254</v>
       </c>
@@ -4013,7 +4014,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="51" t="s">
         <v>256</v>
       </c>
@@ -4031,7 +4032,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="51" t="s">
         <v>258</v>
       </c>
@@ -4049,7 +4050,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="51" t="s">
         <v>262</v>
       </c>
@@ -4067,7 +4068,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="51" t="s">
         <v>264</v>
       </c>
@@ -4085,7 +4086,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="51" t="s">
         <v>304</v>
       </c>
@@ -4103,7 +4104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="51" t="s">
         <v>308</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="51" t="s">
         <v>310</v>
       </c>
@@ -4139,7 +4140,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="51" t="s">
         <v>433</v>
       </c>
@@ -4157,7 +4158,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="51" t="s">
         <v>436</v>
       </c>
@@ -4175,7 +4176,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="51" t="s">
         <v>431</v>
       </c>
@@ -4193,7 +4194,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="51" t="s">
         <v>415</v>
       </c>
@@ -4211,7 +4212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="51" t="s">
         <v>342</v>
       </c>
@@ -4229,7 +4230,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="51" t="s">
         <v>344</v>
       </c>
@@ -4247,7 +4248,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="51" t="s">
         <v>366</v>
       </c>
@@ -4265,7 +4266,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="51" t="s">
         <v>368</v>
       </c>
@@ -4283,7 +4284,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="51" t="s">
         <v>390</v>
       </c>
@@ -4301,7 +4302,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="51" t="s">
         <v>394</v>
       </c>
@@ -4319,7 +4320,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="53" t="s">
         <v>396</v>
       </c>
@@ -4337,7 +4338,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="55" t="s">
         <v>28</v>
       </c>
@@ -4357,7 +4358,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="57" t="s">
         <v>44</v>
       </c>
@@ -4377,7 +4378,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="57" t="s">
         <v>82</v>
       </c>
@@ -4397,7 +4398,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="57" t="s">
         <v>170</v>
       </c>
@@ -4417,7 +4418,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="57" t="s">
         <v>172</v>
       </c>
@@ -4437,7 +4438,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="57" t="s">
         <v>190</v>
       </c>
@@ -4457,7 +4458,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="57" t="s">
         <v>438</v>
       </c>
@@ -4477,7 +4478,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="57" t="s">
         <v>439</v>
       </c>
@@ -4498,7 +4499,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="57" t="s">
         <v>246</v>
       </c>
@@ -4519,7 +4520,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="57" t="s">
         <v>260</v>
       </c>
@@ -4539,7 +4540,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="57" t="s">
         <v>424</v>
       </c>
@@ -4559,7 +4560,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="57" t="s">
         <v>280</v>
       </c>
@@ -4579,7 +4580,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="57" t="s">
         <v>286</v>
       </c>
@@ -4599,7 +4600,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="57" t="s">
         <v>312</v>
       </c>
@@ -4619,7 +4620,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="57" t="s">
         <v>346</v>
       </c>
@@ -4639,7 +4640,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="57" t="s">
         <v>440</v>
       </c>
@@ -4659,7 +4660,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="59" t="s">
         <v>384</v>
       </c>
@@ -4679,7 +4680,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="61" t="s">
         <v>405</v>
       </c>
@@ -4697,7 +4698,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="61" t="s">
         <v>70</v>
       </c>
@@ -4715,7 +4716,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="61" t="s">
         <v>130</v>
       </c>
@@ -4733,7 +4734,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="61" t="s">
         <v>134</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="61" t="s">
         <v>417</v>
       </c>
@@ -4769,7 +4770,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="61" t="s">
         <v>198</v>
       </c>
@@ -4787,7 +4788,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="61" t="s">
         <v>200</v>
       </c>
@@ -4805,7 +4806,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="61" t="s">
         <v>421</v>
       </c>
@@ -4823,7 +4824,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="61" t="s">
         <v>422</v>
       </c>
@@ -4841,7 +4842,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="61" t="s">
         <v>234</v>
       </c>
@@ -4859,7 +4860,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="61" t="s">
         <v>423</v>
       </c>
@@ -4877,7 +4878,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="61" t="s">
         <v>250</v>
       </c>
@@ -4895,7 +4896,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="61" t="s">
         <v>274</v>
       </c>
@@ -4913,7 +4914,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="61" t="s">
         <v>426</v>
       </c>
@@ -4931,7 +4932,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="61" t="s">
         <v>435</v>
       </c>
@@ -4949,7 +4950,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="61" t="s">
         <v>338</v>
       </c>
@@ -4967,7 +4968,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="61" t="s">
         <v>354</v>
       </c>
@@ -4985,7 +4986,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="61" t="s">
         <v>362</v>
       </c>
@@ -5003,7 +5004,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="61" t="s">
         <v>386</v>
       </c>
@@ -5021,7 +5022,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="63" t="s">
         <v>388</v>
       </c>
@@ -5039,7 +5040,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="65" t="s">
         <v>30</v>
       </c>
@@ -5059,7 +5060,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="67" t="s">
         <v>38</v>
       </c>
@@ -5079,7 +5080,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="67" t="s">
         <v>78</v>
       </c>
@@ -5099,7 +5100,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="67" t="s">
         <v>411</v>
       </c>
@@ -5120,7 +5121,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="67" t="s">
         <v>104</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="67" t="s">
         <v>110</v>
       </c>
@@ -5161,7 +5162,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="67" t="s">
         <v>122</v>
       </c>
@@ -5181,7 +5182,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="67" t="s">
         <v>124</v>
       </c>
@@ -5202,7 +5203,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="67" t="s">
         <v>128</v>
       </c>
@@ -5222,7 +5223,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="67" t="s">
         <v>132</v>
       </c>
@@ -5242,7 +5243,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="67" t="s">
         <v>444</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="67" t="s">
         <v>152</v>
       </c>
@@ -5283,7 +5284,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="67" t="s">
         <v>168</v>
       </c>
@@ -5304,7 +5305,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="67" t="s">
         <v>174</v>
       </c>
@@ -5325,7 +5326,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="67" t="s">
         <v>180</v>
       </c>
@@ -5346,7 +5347,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="67" t="s">
         <v>184</v>
       </c>
@@ -5366,7 +5367,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="67" t="s">
         <v>222</v>
       </c>
@@ -5387,7 +5388,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="67" t="s">
         <v>224</v>
       </c>
@@ -5408,7 +5409,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="67" t="s">
         <v>226</v>
       </c>
@@ -5429,7 +5430,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="67" t="s">
         <v>46</v>
       </c>
@@ -5450,7 +5451,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="67" t="s">
         <v>100</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="67" t="s">
         <v>164</v>
       </c>
@@ -5492,7 +5493,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="67" t="s">
         <v>244</v>
       </c>
@@ -5513,7 +5514,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="67" t="s">
         <v>300</v>
       </c>
@@ -5534,7 +5535,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="67" t="s">
         <v>270</v>
       </c>
@@ -5554,7 +5555,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="67" t="s">
         <v>272</v>
       </c>
@@ -5574,7 +5575,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="67" t="s">
         <v>292</v>
       </c>
@@ -5594,7 +5595,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="67" t="s">
         <v>294</v>
       </c>
@@ -5615,7 +5616,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="67" t="s">
         <v>434</v>
       </c>
@@ -5636,7 +5637,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="67" t="s">
         <v>332</v>
       </c>
@@ -5657,7 +5658,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="67" t="s">
         <v>334</v>
       </c>
@@ -5677,7 +5678,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="69" t="s">
         <v>360</v>
       </c>
@@ -5697,7 +5698,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="71" t="s">
         <v>14</v>
       </c>
@@ -5715,7 +5716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="71" t="s">
         <v>404</v>
       </c>
@@ -5733,7 +5734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="71" t="s">
         <v>56</v>
       </c>
@@ -5751,7 +5752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="71" t="s">
         <v>230</v>
       </c>
@@ -5769,7 +5770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="71" t="s">
         <v>425</v>
       </c>
@@ -5787,7 +5788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="71" t="s">
         <v>248</v>
       </c>
@@ -5805,7 +5806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" s="73" t="s">
         <v>322</v>
       </c>
@@ -5823,7 +5824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="75" t="s">
         <v>32</v>
       </c>
@@ -5843,7 +5844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="77" t="s">
         <v>302</v>
       </c>
@@ -5863,7 +5864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="77" t="s">
         <v>192</v>
       </c>
@@ -5883,7 +5884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="79" t="s">
         <v>370</v>
       </c>
@@ -5903,7 +5904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="81" t="s">
         <v>8</v>
       </c>
@@ -5921,7 +5922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="81" t="s">
         <v>22</v>
       </c>
@@ -5939,7 +5940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="81" t="s">
         <v>140</v>
       </c>
@@ -5957,7 +5958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="81" t="s">
         <v>420</v>
       </c>
@@ -5975,7 +5976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="81" t="s">
         <v>348</v>
       </c>
@@ -5993,7 +5994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" s="81" t="s">
         <v>350</v>
       </c>
@@ -6011,7 +6012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A139" s="83" t="s">
         <v>378</v>
       </c>
@@ -6029,7 +6030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" s="85" t="s">
         <v>20</v>
       </c>
@@ -6049,7 +6050,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" s="87" t="s">
         <v>62</v>
       </c>
@@ -6069,7 +6070,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" s="87" t="s">
         <v>80</v>
       </c>
@@ -6089,7 +6090,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" s="87" t="s">
         <v>410</v>
       </c>
@@ -6109,7 +6110,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" s="87" t="s">
         <v>92</v>
       </c>
@@ -6129,7 +6130,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" s="87" t="s">
         <v>116</v>
       </c>
@@ -6149,7 +6150,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="87" t="s">
         <v>236</v>
       </c>
@@ -6169,7 +6170,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="89" t="s">
         <v>284</v>
       </c>
@@ -6189,7 +6190,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="91" t="s">
         <v>401</v>
       </c>
@@ -6207,7 +6208,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="91" t="s">
         <v>402</v>
       </c>
@@ -6225,7 +6226,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="91" t="s">
         <v>403</v>
       </c>
@@ -6243,7 +6244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="91" t="s">
         <v>58</v>
       </c>
@@ -6261,7 +6262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="91" t="s">
         <v>60</v>
       </c>
@@ -6279,7 +6280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="91" t="s">
         <v>64</v>
       </c>
@@ -6297,7 +6298,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="91" t="s">
         <v>108</v>
       </c>
@@ -6315,7 +6316,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="91" t="s">
         <v>412</v>
       </c>
@@ -6333,7 +6334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="91" t="s">
         <v>154</v>
       </c>
@@ -6351,7 +6352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="91" t="s">
         <v>156</v>
       </c>
@@ -6369,7 +6370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="91" t="s">
         <v>158</v>
       </c>
@@ -6387,7 +6388,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="91" t="s">
         <v>162</v>
       </c>
@@ -6405,7 +6406,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="91" t="s">
         <v>166</v>
       </c>
@@ -6423,7 +6424,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="91" t="s">
         <v>186</v>
       </c>
@@ -6441,7 +6442,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="91" t="s">
         <v>428</v>
       </c>
@@ -6459,7 +6460,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="91" t="s">
         <v>429</v>
       </c>
@@ -6477,7 +6478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="91" t="s">
         <v>268</v>
       </c>
@@ -6495,7 +6496,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="91" t="s">
         <v>282</v>
       </c>
@@ -6513,7 +6514,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="91" t="s">
         <v>427</v>
       </c>
@@ -6531,7 +6532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="91" t="s">
         <v>296</v>
       </c>
@@ -6549,7 +6550,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="91" t="s">
         <v>413</v>
       </c>
@@ -6567,7 +6568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="91" t="s">
         <v>328</v>
       </c>
@@ -6585,7 +6586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" s="91" t="s">
         <v>441</v>
       </c>
@@ -6603,7 +6604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="91" t="s">
         <v>372</v>
       </c>
@@ -6621,7 +6622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A172" s="93" t="s">
         <v>430</v>
       </c>
@@ -6639,7 +6640,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="75" t="s">
         <v>442</v>
       </c>
@@ -6659,7 +6660,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="77" t="s">
         <v>418</v>
       </c>
@@ -6679,7 +6680,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="77" t="s">
         <v>178</v>
       </c>
@@ -6699,7 +6700,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="77" t="s">
         <v>182</v>
       </c>
@@ -6719,7 +6720,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" s="77" t="s">
         <v>298</v>
       </c>
@@ -6739,7 +6740,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="79" t="s">
         <v>432</v>
       </c>
@@ -6759,7 +6760,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="81" t="s">
         <v>48</v>
       </c>
@@ -6777,7 +6778,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" s="81" t="s">
         <v>188</v>
       </c>
@@ -6795,7 +6796,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" s="81" t="s">
         <v>206</v>
       </c>
@@ -6813,7 +6814,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A182" s="83" t="s">
         <v>278</v>
       </c>
@@ -6831,7 +6832,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="95" t="s">
         <v>76</v>
       </c>
@@ -6851,7 +6852,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="97" t="s">
         <v>443</v>
       </c>
@@ -6871,7 +6872,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" s="127"/>
       <c r="B185" s="127"/>
       <c r="C185" s="127"/>
@@ -6891,13 +6892,13 @@
       <selection activeCell="A2" sqref="A2:A190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6920,7 +6921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -6947,7 +6948,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -6968,7 +6969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -6995,7 +6996,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -7016,7 +7017,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -7037,7 +7038,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -7064,7 +7065,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -7091,7 +7092,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -7112,7 +7113,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -7133,7 +7134,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -7154,7 +7155,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -7181,7 +7182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -7202,7 +7203,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -7229,7 +7230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -7256,7 +7257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -7277,7 +7278,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -7304,7 +7305,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -7331,7 +7332,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -7358,7 +7359,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -7385,7 +7386,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -7412,7 +7413,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -7439,7 +7440,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -7466,7 +7467,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -7487,7 +7488,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -7514,7 +7515,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -7541,7 +7542,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -7568,7 +7569,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -7595,7 +7596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -7622,7 +7623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -7643,7 +7644,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -7664,7 +7665,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -7685,7 +7686,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -7706,7 +7707,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -7733,7 +7734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -7760,7 +7761,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -7787,7 +7788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -7814,7 +7815,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -7835,7 +7836,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -7862,7 +7863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -7889,7 +7890,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -7916,7 +7917,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -7943,7 +7944,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -7970,7 +7971,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -7991,7 +7992,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -8018,7 +8019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -8045,7 +8046,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -8072,7 +8073,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -8099,7 +8100,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -8120,7 +8121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -8141,7 +8142,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -8162,7 +8163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -8189,7 +8190,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -8210,7 +8211,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>123</v>
       </c>
@@ -8237,7 +8238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>125</v>
       </c>
@@ -8264,7 +8265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -8285,7 +8286,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>129</v>
       </c>
@@ -8312,7 +8313,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>131</v>
       </c>
@@ -8333,7 +8334,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>133</v>
       </c>
@@ -8360,7 +8361,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>135</v>
       </c>
@@ -8387,7 +8388,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>137</v>
       </c>
@@ -8408,7 +8409,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>139</v>
       </c>
@@ -8435,7 +8436,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>141</v>
       </c>
@@ -8462,7 +8463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>143</v>
       </c>
@@ -8489,7 +8490,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>145</v>
       </c>
@@ -8516,7 +8517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>147</v>
       </c>
@@ -8543,7 +8544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -8570,7 +8571,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>151</v>
       </c>
@@ -8597,7 +8598,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -8624,7 +8625,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -8651,7 +8652,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>157</v>
       </c>
@@ -8678,7 +8679,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>159</v>
       </c>
@@ -8705,7 +8706,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>161</v>
       </c>
@@ -8732,7 +8733,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>163</v>
       </c>
@@ -8759,7 +8760,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>165</v>
       </c>
@@ -8786,7 +8787,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>167</v>
       </c>
@@ -8813,7 +8814,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>169</v>
       </c>
@@ -8834,7 +8835,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>171</v>
       </c>
@@ -8855,7 +8856,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>173</v>
       </c>
@@ -8882,7 +8883,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>175</v>
       </c>
@@ -8903,7 +8904,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>177</v>
       </c>
@@ -8930,7 +8931,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>179</v>
       </c>
@@ -8957,7 +8958,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>181</v>
       </c>
@@ -8984,7 +8985,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>183</v>
       </c>
@@ -9005,7 +9006,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>185</v>
       </c>
@@ -9032,7 +9033,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>187</v>
       </c>
@@ -9059,7 +9060,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>189</v>
       </c>
@@ -9080,7 +9081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>191</v>
       </c>
@@ -9107,7 +9108,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>193</v>
       </c>
@@ -9134,7 +9135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>195</v>
       </c>
@@ -9161,7 +9162,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>197</v>
       </c>
@@ -9188,7 +9189,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>199</v>
       </c>
@@ -9215,7 +9216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>201</v>
       </c>
@@ -9242,7 +9243,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>203</v>
       </c>
@@ -9263,7 +9264,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>205</v>
       </c>
@@ -9290,7 +9291,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>207</v>
       </c>
@@ -9317,7 +9318,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>209</v>
       </c>
@@ -9344,7 +9345,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>211</v>
       </c>
@@ -9371,7 +9372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>213</v>
       </c>
@@ -9392,7 +9393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>215</v>
       </c>
@@ -9419,7 +9420,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>217</v>
       </c>
@@ -9446,7 +9447,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>219</v>
       </c>
@@ -9473,7 +9474,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>221</v>
       </c>
@@ -9500,7 +9501,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>223</v>
       </c>
@@ -9527,7 +9528,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>225</v>
       </c>
@@ -9554,7 +9555,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>227</v>
       </c>
@@ -9575,7 +9576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>229</v>
       </c>
@@ -9602,7 +9603,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>231</v>
       </c>
@@ -9629,7 +9630,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>233</v>
       </c>
@@ -9656,7 +9657,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>235</v>
       </c>
@@ -9677,7 +9678,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>237</v>
       </c>
@@ -9704,7 +9705,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>239</v>
       </c>
@@ -9731,7 +9732,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>241</v>
       </c>
@@ -9758,7 +9759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>243</v>
       </c>
@@ -9785,7 +9786,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>245</v>
       </c>
@@ -9812,7 +9813,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>247</v>
       </c>
@@ -9839,7 +9840,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>249</v>
       </c>
@@ -9866,7 +9867,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>251</v>
       </c>
@@ -9893,7 +9894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>253</v>
       </c>
@@ -9920,7 +9921,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>255</v>
       </c>
@@ -9947,7 +9948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>257</v>
       </c>
@@ -9974,7 +9975,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>259</v>
       </c>
@@ -9995,7 +9996,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>261</v>
       </c>
@@ -10022,7 +10023,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>263</v>
       </c>
@@ -10049,7 +10050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>265</v>
       </c>
@@ -10070,7 +10071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>267</v>
       </c>
@@ -10097,7 +10098,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>269</v>
       </c>
@@ -10118,7 +10119,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>271</v>
       </c>
@@ -10139,7 +10140,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>273</v>
       </c>
@@ -10166,7 +10167,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>275</v>
       </c>
@@ -10187,7 +10188,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>277</v>
       </c>
@@ -10214,7 +10215,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>279</v>
       </c>
@@ -10235,7 +10236,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>281</v>
       </c>
@@ -10262,7 +10263,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>283</v>
       </c>
@@ -10283,7 +10284,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>285</v>
       </c>
@@ -10304,7 +10305,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>287</v>
       </c>
@@ -10331,7 +10332,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>289</v>
       </c>
@@ -10358,7 +10359,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>291</v>
       </c>
@@ -10379,7 +10380,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>293</v>
       </c>
@@ -10406,7 +10407,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>295</v>
       </c>
@@ -10433,7 +10434,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>297</v>
       </c>
@@ -10454,7 +10455,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>299</v>
       </c>
@@ -10481,7 +10482,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>301</v>
       </c>
@@ -10502,7 +10503,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>303</v>
       </c>
@@ -10529,7 +10530,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>305</v>
       </c>
@@ -10550,7 +10551,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>307</v>
       </c>
@@ -10577,7 +10578,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>309</v>
       </c>
@@ -10604,7 +10605,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>311</v>
       </c>
@@ -10625,7 +10626,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>313</v>
       </c>
@@ -10652,7 +10653,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>315</v>
       </c>
@@ -10679,7 +10680,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>317</v>
       </c>
@@ -10706,7 +10707,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>319</v>
       </c>
@@ -10733,7 +10734,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>321</v>
       </c>
@@ -10760,7 +10761,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>323</v>
       </c>
@@ -10787,7 +10788,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>325</v>
       </c>
@@ -10814,7 +10815,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>327</v>
       </c>
@@ -10841,7 +10842,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>329</v>
       </c>
@@ -10868,7 +10869,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>331</v>
       </c>
@@ -10895,7 +10896,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>333</v>
       </c>
@@ -10916,7 +10917,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>335</v>
       </c>
@@ -10943,7 +10944,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>337</v>
       </c>
@@ -10970,7 +10971,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>339</v>
       </c>
@@ -10997,7 +10998,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>341</v>
       </c>
@@ -11024,7 +11025,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>343</v>
       </c>
@@ -11051,7 +11052,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>345</v>
       </c>
@@ -11072,7 +11073,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>347</v>
       </c>
@@ -11099,7 +11100,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>349</v>
       </c>
@@ -11126,7 +11127,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>351</v>
       </c>
@@ -11153,7 +11154,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>353</v>
       </c>
@@ -11180,7 +11181,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>355</v>
       </c>
@@ -11207,7 +11208,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>357</v>
       </c>
@@ -11228,7 +11229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>359</v>
       </c>
@@ -11249,7 +11250,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>361</v>
       </c>
@@ -11276,7 +11277,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>363</v>
       </c>
@@ -11297,7 +11298,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>365</v>
       </c>
@@ -11324,7 +11325,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>367</v>
       </c>
@@ -11351,7 +11352,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>369</v>
       </c>
@@ -11372,7 +11373,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>371</v>
       </c>
@@ -11399,7 +11400,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>373</v>
       </c>
@@ -11420,7 +11421,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>375</v>
       </c>
@@ -11444,7 +11445,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>377</v>
       </c>
@@ -11471,7 +11472,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>379</v>
       </c>
@@ -11498,7 +11499,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>381</v>
       </c>
@@ -11525,7 +11526,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>383</v>
       </c>
@@ -11546,7 +11547,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>385</v>
       </c>
@@ -11573,7 +11574,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>387</v>
       </c>
@@ -11600,7 +11601,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>389</v>
       </c>
@@ -11627,7 +11628,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>391</v>
       </c>
@@ -11648,7 +11649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>393</v>
       </c>
@@ -11675,7 +11676,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>395</v>
       </c>
@@ -11716,13 +11717,13 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>451</v>
       </c>
@@ -11733,7 +11734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>453</v>
       </c>
@@ -11744,7 +11745,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>76</v>
       </c>
@@ -11755,7 +11756,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>236</v>
       </c>
@@ -11766,7 +11767,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>62</v>
       </c>
@@ -11777,7 +11778,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>80</v>
       </c>
@@ -11788,7 +11789,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -11799,7 +11800,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>92</v>
       </c>
@@ -11810,7 +11811,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>284</v>
       </c>
@@ -11821,7 +11822,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>116</v>
       </c>
@@ -11832,7 +11833,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>104</v>
       </c>
@@ -11843,7 +11844,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>132</v>
       </c>
@@ -11854,7 +11855,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>455</v>
       </c>
@@ -11865,7 +11866,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>184</v>
       </c>
@@ -11876,7 +11877,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>122</v>
       </c>
@@ -11887,7 +11888,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>270</v>
       </c>
@@ -11898,7 +11899,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>334</v>
       </c>
@@ -11909,7 +11910,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
         <v>292</v>
       </c>
@@ -11920,7 +11921,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>38</v>
       </c>
@@ -11931,7 +11932,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
         <v>30</v>
       </c>
@@ -11942,7 +11943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
         <v>128</v>
       </c>
@@ -11953,7 +11954,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
         <v>272</v>
       </c>
@@ -11964,7 +11965,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
         <v>78</v>
       </c>
@@ -11975,7 +11976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
         <v>360</v>
       </c>
@@ -11986,7 +11987,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
         <v>302</v>
       </c>
@@ -11997,7 +11998,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
         <v>370</v>
       </c>
@@ -12008,7 +12009,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="27" t="s">
         <v>32</v>
       </c>
@@ -12019,7 +12020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="29" t="s">
         <v>306</v>
       </c>
@@ -12030,7 +12031,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="31" t="s">
         <v>418</v>
       </c>
@@ -12041,7 +12042,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="31" t="s">
         <v>442</v>
       </c>
@@ -12052,7 +12053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="31" t="s">
         <v>298</v>
       </c>
@@ -12063,7 +12064,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="34" t="s">
         <v>118</v>
       </c>
@@ -12074,7 +12075,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="36" t="s">
         <v>114</v>
       </c>
@@ -12085,7 +12086,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="36" t="s">
         <v>12</v>
       </c>
@@ -12096,7 +12097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="36" t="s">
         <v>228</v>
       </c>
@@ -12107,7 +12108,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="36" t="s">
         <v>266</v>
       </c>
@@ -12118,7 +12119,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
         <v>214</v>
       </c>
@@ -12129,7 +12130,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="36" t="s">
         <v>392</v>
       </c>
@@ -12140,7 +12141,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="38" t="s">
         <v>358</v>
       </c>
@@ -12151,7 +12152,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>82</v>
       </c>
@@ -12162,7 +12163,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>172</v>
       </c>
@@ -12173,7 +12174,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>280</v>
       </c>
@@ -12184,7 +12185,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>44</v>
       </c>
@@ -12195,7 +12196,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>440</v>
       </c>
@@ -12206,7 +12207,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>170</v>
       </c>
@@ -12217,7 +12218,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>260</v>
       </c>
@@ -12228,7 +12229,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>346</v>
       </c>
@@ -12239,7 +12240,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>384</v>
       </c>
@@ -12250,7 +12251,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>286</v>
       </c>
@@ -12261,7 +12262,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>312</v>
       </c>
@@ -12272,7 +12273,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>190</v>
       </c>
@@ -12283,7 +12284,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>456</v>
       </c>
@@ -12294,7 +12295,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>28</v>
       </c>
@@ -12305,7 +12306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="40" t="s">
         <v>276</v>
       </c>
@@ -12316,134 +12317,134 @@
         <v>275</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="41"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="41"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="41"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="41"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="41"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="41"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="41"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="41"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="41"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="41"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="41"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="41"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="41"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="41"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="41"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="41"/>
       <c r="B101" s="41"/>
       <c r="C101" s="41"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="41"/>
       <c r="B102" s="41"/>
       <c r="C102" s="41"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="41"/>
       <c r="B108" s="41"/>
       <c r="C108" s="41"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="41"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="41"/>
       <c r="B118" s="41"/>
       <c r="C118" s="41"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="41"/>
       <c r="B119" s="41"/>
       <c r="C119" s="41"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="41"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="41"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="41"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="41"/>
       <c r="B124" s="41"/>
       <c r="C124" s="41"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="41"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="41"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="41"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="41"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="41"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" s="41"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="41"/>
       <c r="B163" s="41"/>
       <c r="C163" s="41"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="41"/>
       <c r="B164" s="41"/>
       <c r="C164" s="41"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="41"/>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="41"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" s="41"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" s="41"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" s="41"/>
     </row>
   </sheetData>

</xml_diff>